<commit_message>
Added Water Change logic
</commit_message>
<xml_diff>
--- a/docs/NuevaPantalla.xlsx
+++ b/docs/NuevaPantalla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vsanz/CloudStation/Dev/aquarium_care_by_arduino/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04D41D9-F746-4F45-88C2-E88FB3EFDA18}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A13EAF-6400-564F-8A79-DB5C41D1822B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="14480" windowHeight="15120" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="460" windowWidth="24820" windowHeight="19640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lumens" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,17 @@
     <sheet name="Arduino" sheetId="4" r:id="rId4"/>
     <sheet name="Screens" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Design!$C$4:$V$20</definedName>
+  </definedNames>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -2526,8 +2535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AR42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2:Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5422,7 +5431,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -5778,7 +5787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
@@ -6669,16 +6678,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A26:Q26"/>
+    <mergeCell ref="A10:Q10"/>
+    <mergeCell ref="A38:Q38"/>
+    <mergeCell ref="A30:Q30"/>
+    <mergeCell ref="A34:Q34"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A6:Q6"/>
     <mergeCell ref="A14:Q14"/>
     <mergeCell ref="A18:Q18"/>
     <mergeCell ref="A22:Q22"/>
-    <mergeCell ref="A26:Q26"/>
-    <mergeCell ref="A10:Q10"/>
-    <mergeCell ref="A38:Q38"/>
-    <mergeCell ref="A30:Q30"/>
-    <mergeCell ref="A34:Q34"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Print i2c devices while setup
</commit_message>
<xml_diff>
--- a/docs/NuevaPantalla.xlsx
+++ b/docs/NuevaPantalla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vsanz/CloudStation/Dev/aquarium_care_by_arduino/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A13EAF-6400-564F-8A79-DB5C41D1822B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152898E7-C1E1-0D47-8E69-F36093C8D8C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="460" windowWidth="24820" windowHeight="19640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2536,7 +2536,7 @@
   <dimension ref="A1:AR42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:Z2"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3919,58 +3919,58 @@
         <v>2</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
         <v>2</v>
-      </c>
-      <c r="V17">
-        <v>1</v>
       </c>
       <c r="X17" s="29">
         <f t="shared" si="5"/>
@@ -4022,46 +4022,46 @@
     </row>
     <row r="18" spans="2:43" x14ac:dyDescent="0.2">
       <c r="C18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
         <v>4</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>3</v>
       </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
       <c r="J18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
         <v>3</v>
       </c>
-      <c r="M18">
-        <v>2</v>
-      </c>
       <c r="N18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q18">
         <v>3</v>
@@ -4070,16 +4070,16 @@
         <v>4</v>
       </c>
       <c r="S18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="V18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X18" s="29">
         <f t="shared" si="5"/>
@@ -4131,16 +4131,16 @@
     </row>
     <row r="19" spans="2:43" x14ac:dyDescent="0.2">
       <c r="C19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -4149,46 +4149,46 @@
         <v>6</v>
       </c>
       <c r="I19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M19">
         <v>5</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
         <v>6</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>5</v>
       </c>
-      <c r="S19">
-        <v>4</v>
-      </c>
       <c r="T19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X19" s="29">
         <f t="shared" si="5"/>
@@ -4240,58 +4240,58 @@
     </row>
     <row r="20" spans="2:43" x14ac:dyDescent="0.2">
       <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>7</v>
       </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
       <c r="F20">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M20">
+        <v>7</v>
+      </c>
+      <c r="N20">
         <v>8</v>
       </c>
-      <c r="N20">
-        <v>6</v>
-      </c>
       <c r="O20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="T20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U20">
         <v>7</v>
@@ -6678,16 +6678,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A6:Q6"/>
+    <mergeCell ref="A14:Q14"/>
+    <mergeCell ref="A18:Q18"/>
+    <mergeCell ref="A22:Q22"/>
     <mergeCell ref="A26:Q26"/>
     <mergeCell ref="A10:Q10"/>
     <mergeCell ref="A38:Q38"/>
     <mergeCell ref="A30:Q30"/>
     <mergeCell ref="A34:Q34"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A6:Q6"/>
-    <mergeCell ref="A14:Q14"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="A22:Q22"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>